<commit_message>
Fixed BAU Deaths by Demographic Trait; assigned hispanic ethnicity to race based on data from CA (previously this was erroneously all going to "other", but the vast majority is "white" per CA data
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/FoPITY/Supporting Calculations for Policy Schedules.xlsx
+++ b/InputData/plcy-schd/FoPITY/Supporting Calculations for Policy Schedules.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\plcy-schd\FoPITY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\plcy-schd\FoPITY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7300916-EA8E-48F2-A9A1-CEF97C48C667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6282821C-1FA2-4323-BF68-8A3585FF4719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10515" yWindow="240" windowWidth="27855" windowHeight="21855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
     <sheet name="Exogenous GDP Adjustment" sheetId="6" r:id="rId2"/>
     <sheet name="R&amp;D Policies" sheetId="2" r:id="rId3"/>
+    <sheet name="EV Standard" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="final_year">'R&amp;D Policies'!#REF!</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>Year</t>
   </si>
@@ -175,6 +176,57 @@
   </si>
   <si>
     <t>in case the user wishes to use the Mandated Capacity Construction Schedule</t>
+  </si>
+  <si>
+    <t>Time (Time)</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[LDVs,passenger] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[LDVs,freight] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[HDVs,passenger] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[HDVs,freight] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[aircraft,passenger] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[aircraft,freight] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[rail,passenger] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[rail,freight] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[ships,passenger] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[ships,freight] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[motorbikes,passenger] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>BMRESP BAU Minimum Required EV Sales Percentage[motorbikes,freight] : MostRecentRun</t>
+  </si>
+  <si>
+    <t>Policy Commitments</t>
+  </si>
+  <si>
+    <t>Deeper Decarbonization</t>
+  </si>
+  <si>
+    <t>Policy Values</t>
+  </si>
+  <si>
+    <t>Policy Schedules</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8D652C-DDA1-4972-BD18-A83039143417}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3287,4 +3339,1751 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F6D8E8-A2F3-4C1A-A2CA-9AB629B8B97C}">
+  <dimension ref="A1:AF21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W32" sqref="W32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="87.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1">
+        <v>2020</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2022</v>
+      </c>
+      <c r="E1">
+        <v>2023</v>
+      </c>
+      <c r="F1">
+        <v>2024</v>
+      </c>
+      <c r="G1">
+        <v>2025</v>
+      </c>
+      <c r="H1">
+        <v>2026</v>
+      </c>
+      <c r="I1">
+        <v>2027</v>
+      </c>
+      <c r="J1">
+        <v>2028</v>
+      </c>
+      <c r="K1">
+        <v>2029</v>
+      </c>
+      <c r="L1">
+        <v>2030</v>
+      </c>
+      <c r="M1">
+        <v>2031</v>
+      </c>
+      <c r="N1">
+        <v>2032</v>
+      </c>
+      <c r="O1">
+        <v>2033</v>
+      </c>
+      <c r="P1">
+        <v>2034</v>
+      </c>
+      <c r="Q1">
+        <v>2035</v>
+      </c>
+      <c r="R1">
+        <v>2036</v>
+      </c>
+      <c r="S1">
+        <v>2037</v>
+      </c>
+      <c r="T1">
+        <v>2038</v>
+      </c>
+      <c r="U1">
+        <v>2039</v>
+      </c>
+      <c r="V1">
+        <v>2040</v>
+      </c>
+      <c r="W1">
+        <v>2041</v>
+      </c>
+      <c r="X1">
+        <v>2042</v>
+      </c>
+      <c r="Y1">
+        <v>2043</v>
+      </c>
+      <c r="Z1">
+        <v>2044</v>
+      </c>
+      <c r="AA1">
+        <v>2045</v>
+      </c>
+      <c r="AB1">
+        <v>2046</v>
+      </c>
+      <c r="AC1">
+        <v>2047</v>
+      </c>
+      <c r="AD1">
+        <v>2048</v>
+      </c>
+      <c r="AE1">
+        <v>2049</v>
+      </c>
+      <c r="AF1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>4.2396200000000002E-2</v>
+      </c>
+      <c r="C2">
+        <v>5.0699800000000003E-2</v>
+      </c>
+      <c r="D2">
+        <v>5.6578499999999997E-2</v>
+      </c>
+      <c r="E2">
+        <v>6.3298099999999996E-2</v>
+      </c>
+      <c r="F2">
+        <v>6.9598300000000002E-2</v>
+      </c>
+      <c r="G2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="H2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="I2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="J2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="K2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="L2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="M2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="N2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="O2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="P2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="Q2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="R2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="S2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="T2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="U2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="V2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="W2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="X2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="Y2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="Z2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="AA2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="AB2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="AC2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="AD2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="AE2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+      <c r="AF2">
+        <v>7.5536099999999995E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>5.5031900000000002E-2</v>
+      </c>
+      <c r="G3">
+        <v>7.3761699999999999E-2</v>
+      </c>
+      <c r="H3">
+        <v>9.9696699999999999E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.15063499999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.20788300000000001</v>
+      </c>
+      <c r="K3">
+        <v>0.26519799999999999</v>
+      </c>
+      <c r="L3">
+        <v>0.32253900000000002</v>
+      </c>
+      <c r="M3">
+        <v>0.36920900000000001</v>
+      </c>
+      <c r="N3">
+        <v>0.41588000000000003</v>
+      </c>
+      <c r="O3">
+        <v>0.46255000000000002</v>
+      </c>
+      <c r="P3">
+        <v>0.50922000000000001</v>
+      </c>
+      <c r="Q3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="R3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="S3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="T3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="U3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="V3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="W3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="X3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="Y3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="Z3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="AA3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="AB3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="AC3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="AD3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="AE3">
+        <v>0.55589100000000002</v>
+      </c>
+      <c r="AF3">
+        <v>0.55589100000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>7.6549500000000006E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.138992</v>
+      </c>
+      <c r="G4">
+        <v>0.152868</v>
+      </c>
+      <c r="H4">
+        <v>0.24329300000000001</v>
+      </c>
+      <c r="I4">
+        <v>0.29185899999999998</v>
+      </c>
+      <c r="J4">
+        <v>0.36124000000000001</v>
+      </c>
+      <c r="K4">
+        <v>0.58371899999999999</v>
+      </c>
+      <c r="L4">
+        <v>0.65309899999999999</v>
+      </c>
+      <c r="M4">
+        <v>0.68778899999999998</v>
+      </c>
+      <c r="N4">
+        <v>0.72247899999999998</v>
+      </c>
+      <c r="O4">
+        <v>0.75716899999999998</v>
+      </c>
+      <c r="P4">
+        <v>0.79185899999999998</v>
+      </c>
+      <c r="Q4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="R4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="S4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="T4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="U4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="V4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="W4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="X4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="Y4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="Z4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="AA4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="AB4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="AC4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="AD4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="AE4">
+        <v>0.82654899999999998</v>
+      </c>
+      <c r="AF4">
+        <v>0.82654899999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.05</v>
+      </c>
+      <c r="G5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
+        <v>0.15</v>
+      </c>
+      <c r="J5">
+        <v>0.2</v>
+      </c>
+      <c r="K5">
+        <v>0.25</v>
+      </c>
+      <c r="L5">
+        <v>0.3</v>
+      </c>
+      <c r="M5">
+        <v>0.35</v>
+      </c>
+      <c r="N5">
+        <v>0.4</v>
+      </c>
+      <c r="O5">
+        <v>0.4</v>
+      </c>
+      <c r="P5">
+        <v>0.4</v>
+      </c>
+      <c r="Q5">
+        <v>0.4</v>
+      </c>
+      <c r="R5">
+        <v>0.4</v>
+      </c>
+      <c r="S5">
+        <v>0.4</v>
+      </c>
+      <c r="T5">
+        <v>0.4</v>
+      </c>
+      <c r="U5">
+        <v>0.4</v>
+      </c>
+      <c r="V5">
+        <v>0.4</v>
+      </c>
+      <c r="W5">
+        <v>0.4</v>
+      </c>
+      <c r="X5">
+        <v>0.4</v>
+      </c>
+      <c r="Y5">
+        <v>0.4</v>
+      </c>
+      <c r="Z5">
+        <v>0.4</v>
+      </c>
+      <c r="AA5">
+        <v>0.4</v>
+      </c>
+      <c r="AB5">
+        <v>0.4</v>
+      </c>
+      <c r="AC5">
+        <v>0.4</v>
+      </c>
+      <c r="AD5">
+        <v>0.4</v>
+      </c>
+      <c r="AE5">
+        <v>0.4</v>
+      </c>
+      <c r="AF5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0.05</v>
+      </c>
+      <c r="G13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H13">
+        <v>0.1</v>
+      </c>
+      <c r="I13">
+        <v>0.15</v>
+      </c>
+      <c r="J13">
+        <v>0.2</v>
+      </c>
+      <c r="K13">
+        <v>0.25</v>
+      </c>
+      <c r="L13">
+        <v>0.3</v>
+      </c>
+      <c r="M13">
+        <v>0.35</v>
+      </c>
+      <c r="N13">
+        <v>0.4</v>
+      </c>
+      <c r="O13">
+        <v>0.4</v>
+      </c>
+      <c r="P13">
+        <v>0.4</v>
+      </c>
+      <c r="Q13">
+        <v>0.4</v>
+      </c>
+      <c r="R13">
+        <v>0.4</v>
+      </c>
+      <c r="S13">
+        <v>0.4</v>
+      </c>
+      <c r="T13">
+        <v>0.4</v>
+      </c>
+      <c r="U13">
+        <v>0.4</v>
+      </c>
+      <c r="V13">
+        <v>0.4</v>
+      </c>
+      <c r="W13">
+        <v>0.4</v>
+      </c>
+      <c r="X13">
+        <v>0.4</v>
+      </c>
+      <c r="Y13">
+        <v>0.4</v>
+      </c>
+      <c r="Z13">
+        <v>0.4</v>
+      </c>
+      <c r="AA13">
+        <v>0.4</v>
+      </c>
+      <c r="AB13">
+        <v>0.4</v>
+      </c>
+      <c r="AC13">
+        <v>0.4</v>
+      </c>
+      <c r="AD13">
+        <v>0.4</v>
+      </c>
+      <c r="AE13">
+        <v>0.4</v>
+      </c>
+      <c r="AF13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16">
+        <f>$V$16/COUNT($E$1:$V$1)*(E$1-$D$1)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:U16" si="0">$V$16/COUNT($E$1:$V$1)*(F$1-$D$1)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="0"/>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="V16">
+        <v>0.6</v>
+      </c>
+      <c r="W16">
+        <v>0.6</v>
+      </c>
+      <c r="X16">
+        <v>0.6</v>
+      </c>
+      <c r="Y16">
+        <v>0.6</v>
+      </c>
+      <c r="Z16">
+        <v>0.6</v>
+      </c>
+      <c r="AA16">
+        <v>0.6</v>
+      </c>
+      <c r="AB16">
+        <v>0.6</v>
+      </c>
+      <c r="AC16">
+        <v>0.6</v>
+      </c>
+      <c r="AD16">
+        <v>0.6</v>
+      </c>
+      <c r="AE16">
+        <v>0.6</v>
+      </c>
+      <c r="AF16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17">
+        <f>$Q$17/COUNT($E$1:$Q$1)*(E$1-$D$1)</f>
+        <v>4.6153846153846149E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:P17" si="1">$Q$17/COUNT($E$1:$Q$1)*(F$1-$D$1)</f>
+        <v>9.2307692307692299E-2</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0.13846153846153844</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>0.1846153846153846</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0.23076923076923075</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>0.27692307692307688</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>0.32307692307692304</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>0.3692307692307692</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>0.41538461538461535</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>0.46153846153846151</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="1"/>
+        <v>0.50769230769230766</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="1"/>
+        <v>0.55384615384615377</v>
+      </c>
+      <c r="Q17">
+        <v>0.6</v>
+      </c>
+      <c r="R17">
+        <f>Q17</f>
+        <v>0.6</v>
+      </c>
+      <c r="S17">
+        <f t="shared" ref="S17:AF17" si="2">R17</f>
+        <v>0.6</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="AE17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="AF17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20">
+        <f>E16/$AF16</f>
+        <v>5.5555555555555559E-2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ref="F20:U20" si="3">F16/$AF16</f>
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>0.22222222222222224</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="3"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="3"/>
+        <v>0.44444444444444448</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="3"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="3"/>
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="3"/>
+        <v>0.72222222222222232</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="3"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="3"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="3"/>
+        <v>0.88888888888888895</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="3"/>
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+      <c r="AD20">
+        <v>1</v>
+      </c>
+      <c r="AE20">
+        <v>1</v>
+      </c>
+      <c r="AF20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21">
+        <f>E17/$AF17</f>
+        <v>7.6923076923076913E-2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21:AF21" si="4">F17/$AF17</f>
+        <v>0.15384615384615383</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>0.23076923076923075</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>0.30769230769230765</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>0.38461538461538458</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="4"/>
+        <v>0.46153846153846151</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="4"/>
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="4"/>
+        <v>0.61538461538461531</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="4"/>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="4"/>
+        <v>0.76923076923076916</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="4"/>
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="4"/>
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AB21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AC21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AE21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>